<commit_message>
fixing characteristic names in completeness file, messing with vignettee unicode
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleDQOCompleteness_final.xlsx
+++ b/inst/extdata/ExampleDQOCompleteness_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6A4877-E62D-49E1-8161-9F099DE88472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662323AC-169F-49B8-B8D5-4350A03C2C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31200" yWindow="945" windowWidth="19455" windowHeight="9315" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
@@ -64,12 +64,6 @@
     <t>TP</t>
   </si>
   <si>
-    <t>NO3</t>
-  </si>
-  <si>
-    <t>NH3</t>
-  </si>
-  <si>
     <t>Chloride</t>
   </si>
   <si>
@@ -92,6 +86,12 @@
   </si>
   <si>
     <t>Chl a</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G2"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,14 +536,14 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -557,10 +557,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>3</v>
@@ -578,13 +578,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" s="6">
         <v>90</v>
@@ -601,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6">
         <v>10</v>
@@ -624,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6">
         <v>10</v>
@@ -647,7 +647,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="6">
         <v>10</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="6">
         <v>10</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B10" s="6">
         <v>10</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6">
         <v>10</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="6">
         <v>10</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="6">
         <v>10</v>

</xml_diff>